<commit_message>
sua file import thiet bi
</commit_message>
<xml_diff>
--- a/web/uploads/excel/down/mau_import_tai_san.xlsx
+++ b/web/uploads/excel/down/mau_import_tai_san.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AN\Desktop\qlts-test\web\uploads\excel\down\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CV\2025\QLTS2\qlts.v2\web\uploads\excel\down\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DC13BB-EDE0-479B-8604-65945D2B6A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B237D2B-3A56-4E82-90A9-CCA92FA1B211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>STT</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Thông tin quản lý</t>
+  </si>
+  <si>
+    <t>Số khung</t>
+  </si>
+  <si>
+    <t>Số máy</t>
+  </si>
+  <si>
+    <t>Xe</t>
   </si>
 </sst>
 </file>
@@ -289,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -303,6 +312,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -312,21 +330,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,22 +622,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W10"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="AB14" sqref="AB14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -649,39 +663,45 @@
       <c r="U1" s="12"/>
       <c r="V1" s="12"/>
       <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="5" t="s">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="B2" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="5" t="s">
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="7"/>
-      <c r="N2" s="5" t="s">
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="7"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="9"/>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
       <c r="W2" s="10"/>
+      <c r="X2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="14"/>
     </row>
-    <row r="3" spans="1:23" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" s="2" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -697,7 +717,7 @@
       <c r="E3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="7" t="s">
         <v>18</v>
       </c>
       <c r="G3" s="3" t="s">
@@ -721,16 +741,16 @@
       <c r="M3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="13" t="s">
+      <c r="N3" s="7" t="s">
         <v>33</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="P3" s="13" t="s">
+      <c r="P3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="7" t="s">
         <v>35</v>
       </c>
       <c r="R3" s="3" t="s">
@@ -751,9 +771,15 @@
       <c r="W3" s="3" t="s">
         <v>41</v>
       </c>
+      <c r="X3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
+    <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -796,9 +822,11 @@
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
+      <c r="X4" s="4"/>
+      <c r="Y4" s="4"/>
     </row>
-    <row r="5" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8">
+    <row r="5" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -839,9 +867,11 @@
       <c r="U5" s="4"/>
       <c r="V5" s="4"/>
       <c r="W5" s="4"/>
+      <c r="X5" s="4"/>
+      <c r="Y5" s="4"/>
     </row>
-    <row r="6" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8">
+    <row r="6" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -884,9 +914,11 @@
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
+      <c r="X6" s="4"/>
+      <c r="Y6" s="4"/>
     </row>
-    <row r="7" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
+    <row r="7" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -929,9 +961,11 @@
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
     </row>
-    <row r="8" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="8">
+    <row r="8" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -972,9 +1006,11 @@
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
     </row>
-    <row r="9" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="8">
+    <row r="9" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1015,9 +1051,11 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
+      <c r="X9" s="4"/>
+      <c r="Y9" s="4"/>
     </row>
-    <row r="10" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
+    <row r="10" spans="1:25" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
@@ -1056,13 +1094,16 @@
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
+      <c r="X10" s="4"/>
+      <c r="Y10" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
+    <mergeCell ref="X2:Y2"/>
+    <mergeCell ref="A1:Y1"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="J2:M2"/>
-    <mergeCell ref="N2:V2"/>
-    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="N2:W2"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>